<commit_message>
I added clear button
</commit_message>
<xml_diff>
--- a/Publications.xlsx
+++ b/Publications.xlsx
@@ -487,7 +487,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3">
@@ -577,7 +577,7 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12">
@@ -587,7 +587,7 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13">
@@ -627,7 +627,7 @@
         </is>
       </c>
       <c r="B16" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17">
@@ -647,7 +647,7 @@
         </is>
       </c>
       <c r="B18" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19">
@@ -737,7 +737,7 @@
         </is>
       </c>
       <c r="B27" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28">
@@ -757,7 +757,7 @@
         </is>
       </c>
       <c r="B29" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30">
@@ -777,7 +777,7 @@
         </is>
       </c>
       <c r="B31" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32">
@@ -787,7 +787,7 @@
         </is>
       </c>
       <c r="B32" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33">
@@ -797,7 +797,7 @@
         </is>
       </c>
       <c r="B33" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34">
@@ -807,7 +807,7 @@
         </is>
       </c>
       <c r="B34" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35">
@@ -847,7 +847,7 @@
         </is>
       </c>
       <c r="B38" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39">
@@ -867,7 +867,7 @@
         </is>
       </c>
       <c r="B40" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41">
@@ -887,7 +887,7 @@
         </is>
       </c>
       <c r="B42" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43">
@@ -927,7 +927,7 @@
         </is>
       </c>
       <c r="B46" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47">
@@ -1007,7 +1007,7 @@
         </is>
       </c>
       <c r="B54" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55">
@@ -1027,7 +1027,7 @@
         </is>
       </c>
       <c r="B56" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57">
@@ -1037,7 +1037,7 @@
         </is>
       </c>
       <c r="B57" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58">
@@ -1077,7 +1077,7 @@
         </is>
       </c>
       <c r="B61" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62">
@@ -1087,7 +1087,7 @@
         </is>
       </c>
       <c r="B62" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63">
@@ -1097,7 +1097,7 @@
         </is>
       </c>
       <c r="B63" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="64">
@@ -1117,7 +1117,7 @@
         </is>
       </c>
       <c r="B65" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="66">
@@ -1137,7 +1137,7 @@
         </is>
       </c>
       <c r="B67" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68">
@@ -1167,7 +1167,7 @@
         </is>
       </c>
       <c r="B70" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71">
@@ -1357,7 +1357,7 @@
         </is>
       </c>
       <c r="B89" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="90">
@@ -1377,7 +1377,7 @@
         </is>
       </c>
       <c r="B91" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="92">
@@ -1387,7 +1387,7 @@
         </is>
       </c>
       <c r="B92" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="93">
@@ -1447,7 +1447,7 @@
         </is>
       </c>
       <c r="B98" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="99">
@@ -1527,7 +1527,7 @@
         </is>
       </c>
       <c r="B106" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="107">
@@ -1537,7 +1537,7 @@
         </is>
       </c>
       <c r="B107" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="108">
@@ -1567,7 +1567,7 @@
         </is>
       </c>
       <c r="B110" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="111">
@@ -1577,7 +1577,7 @@
         </is>
       </c>
       <c r="B111" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="112">

</xml_diff>